<commit_message>
Read excel file and add numbers to list
</commit_message>
<xml_diff>
--- a/dane.xlsx
+++ b/dane.xlsx
@@ -8,17 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Ekonometry\Ekonometry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A2C7B27-CD7F-4D7A-BD49-FA520CC3000C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0FB59C-5A37-472F-8887-E233211D64ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37050" yWindow="1380" windowWidth="13890" windowHeight="13650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="date" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -49,7 +58,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.#0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -60,6 +69,12 @@
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
     </font>
   </fonts>
   <fills count="2">
@@ -98,7 +113,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -110,6 +125,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -394,7 +415,7 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="A2" sqref="A2:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,200 +439,205 @@
       <c r="F1" s="4"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>0.87</v>
+      <c r="A2" s="5">
+        <f>0.87*10^3</f>
+        <v>870</v>
       </c>
       <c r="B2" s="1">
-        <v>0.82</v>
+        <f>0.82*10^3</f>
+        <v>820</v>
       </c>
       <c r="C2" s="2">
         <v>674.8</v>
       </c>
       <c r="D2" s="1">
-        <v>3315.38</v>
-      </c>
-      <c r="E2" s="3">
-        <v>488898</v>
+        <v>331.53800000000001</v>
+      </c>
+      <c r="E2" s="6">
+        <v>488.89800000000002</v>
       </c>
       <c r="F2" s="4"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>0.87</v>
+        <f>0.87*10^3</f>
+        <v>870</v>
       </c>
       <c r="B3" s="1">
-        <v>0.82</v>
+        <v>820</v>
       </c>
       <c r="C3" s="2">
         <v>717.8</v>
       </c>
       <c r="D3" s="1">
-        <v>3435</v>
-      </c>
-      <c r="E3" s="3">
-        <v>568687</v>
+        <v>343.5</v>
+      </c>
+      <c r="E3" s="6">
+        <v>568.68700000000001</v>
       </c>
       <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>0.86</v>
+        <f>0.86*10^3</f>
+        <v>860</v>
       </c>
       <c r="B4" s="1">
-        <v>0.81</v>
+        <v>810</v>
       </c>
       <c r="C4" s="2">
         <v>694.1</v>
       </c>
       <c r="D4" s="1">
-        <v>3625.21</v>
-      </c>
-      <c r="E4" s="3">
-        <v>685237</v>
+        <f>3625.21*10^-1</f>
+        <v>362.52100000000002</v>
+      </c>
+      <c r="E4" s="6">
+        <v>685.23699999999997</v>
       </c>
       <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>0.83</v>
+        <v>830</v>
       </c>
       <c r="B5" s="1">
-        <v>0.8</v>
+        <v>800</v>
       </c>
       <c r="C5" s="2">
         <v>618.70000000000005</v>
       </c>
       <c r="D5" s="1">
-        <v>3744.38</v>
-      </c>
-      <c r="E5" s="3">
-        <v>757239</v>
+        <v>374.43799999999999</v>
+      </c>
+      <c r="E5" s="6">
+        <v>757.23900000000003</v>
       </c>
       <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>0.82</v>
+        <v>820</v>
       </c>
       <c r="B6" s="1">
-        <v>0.79</v>
+        <v>790</v>
       </c>
       <c r="C6" s="2">
         <v>595.79999999999995</v>
       </c>
       <c r="D6" s="1">
-        <v>3877.43</v>
-      </c>
-      <c r="E6" s="3">
-        <v>827080</v>
+        <v>387.74299999999999</v>
+      </c>
+      <c r="E6" s="6">
+        <v>827.08</v>
       </c>
       <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>0.79</v>
+        <v>790</v>
       </c>
       <c r="B7" s="1">
-        <v>0.78</v>
+        <v>780</v>
       </c>
       <c r="C7" s="2">
         <v>614.79999999999995</v>
       </c>
       <c r="D7" s="1">
-        <v>4003.99</v>
-      </c>
-      <c r="E7" s="3">
-        <v>760056</v>
+        <v>400.399</v>
+      </c>
+      <c r="E7" s="6">
+        <v>760.05600000000004</v>
       </c>
       <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>0.77</v>
+        <v>770</v>
       </c>
       <c r="B8" s="1">
-        <v>0.78</v>
+        <v>780</v>
       </c>
       <c r="C8" s="2">
         <v>502.4</v>
       </c>
       <c r="D8" s="1">
-        <v>4150.8599999999997</v>
-      </c>
-      <c r="E8" s="3">
-        <v>620855</v>
+        <v>415.08600000000001</v>
+      </c>
+      <c r="E8" s="6">
+        <v>620.85500000000002</v>
       </c>
       <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
-        <v>0.55000000000000004</v>
+        <v>550</v>
       </c>
       <c r="B9" s="1">
-        <v>0.99</v>
+        <v>990</v>
       </c>
       <c r="C9" s="2">
         <v>465</v>
       </c>
       <c r="D9" s="1">
-        <v>4290.5200000000004</v>
-      </c>
-      <c r="E9" s="3">
-        <v>542843</v>
+        <v>429.05200000000002</v>
+      </c>
+      <c r="E9" s="6">
+        <v>542.84299999999996</v>
       </c>
       <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
-        <v>0.36</v>
+        <v>360</v>
       </c>
       <c r="B10" s="1">
-        <v>1.1599999999999999</v>
+        <v>1160</v>
       </c>
       <c r="C10" s="2">
         <v>580.29999999999995</v>
       </c>
       <c r="D10" s="1">
-        <v>4527.8900000000003</v>
-      </c>
-      <c r="E10" s="3">
-        <v>438404</v>
+        <v>452.78899999999999</v>
+      </c>
+      <c r="E10" s="6">
+        <v>438.404</v>
       </c>
       <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>0.34</v>
+        <v>340</v>
       </c>
       <c r="B11" s="1">
-        <v>1.18</v>
+        <v>1180</v>
       </c>
       <c r="C11" s="2">
         <v>609.29999999999995</v>
       </c>
       <c r="D11" s="1">
-        <v>4834.76</v>
-      </c>
-      <c r="E11" s="3">
-        <v>383301</v>
+        <v>483.476</v>
+      </c>
+      <c r="E11" s="6">
+        <v>383.30099999999999</v>
       </c>
       <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
-        <v>0.64</v>
+        <v>640</v>
       </c>
       <c r="B12" s="1">
-        <v>0.87</v>
+        <v>870</v>
       </c>
       <c r="C12" s="2">
         <v>521.6</v>
       </c>
       <c r="D12" s="1">
-        <v>5181.63</v>
-      </c>
-      <c r="E12" s="3">
-        <v>328880</v>
+        <v>518.16300000000001</v>
+      </c>
+      <c r="E12" s="6">
+        <v>328.88</v>
       </c>
       <c r="F12" s="4"/>
     </row>

</xml_diff>

<commit_message>
Make file browers connected with button
</commit_message>
<xml_diff>
--- a/dane.xlsx
+++ b/dane.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Ekonometry\Ekonometry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B0FB59C-5A37-472F-8887-E233211D64ED}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A40266D-2479-4EF8-8362-CB561DA7624B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13740" yWindow="1950" windowWidth="13890" windowHeight="13650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="date" sheetId="1" r:id="rId1"/>
@@ -113,7 +113,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -121,14 +121,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -415,31 +418,31 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E12"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4"/>
+      <c r="F1" s="3"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <f>0.87*10^3</f>
         <v>870</v>
       </c>
@@ -453,10 +456,10 @@
       <c r="D2" s="1">
         <v>331.53800000000001</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="5">
         <v>488.89800000000002</v>
       </c>
-      <c r="F2" s="4"/>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
@@ -472,10 +475,10 @@
       <c r="D3" s="1">
         <v>343.5</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>568.68700000000001</v>
       </c>
-      <c r="F3" s="4"/>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
@@ -492,10 +495,10 @@
         <f>3625.21*10^-1</f>
         <v>362.52100000000002</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>685.23699999999997</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
@@ -510,10 +513,10 @@
       <c r="D5" s="1">
         <v>374.43799999999999</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>757.23900000000003</v>
       </c>
-      <c r="F5" s="4"/>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
@@ -528,10 +531,10 @@
       <c r="D6" s="1">
         <v>387.74299999999999</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>827.08</v>
       </c>
-      <c r="F6" s="4"/>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -546,10 +549,10 @@
       <c r="D7" s="1">
         <v>400.399</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>760.05600000000004</v>
       </c>
-      <c r="F7" s="4"/>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
@@ -564,10 +567,10 @@
       <c r="D8" s="1">
         <v>415.08600000000001</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>620.85500000000002</v>
       </c>
-      <c r="F8" s="4"/>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
@@ -582,10 +585,10 @@
       <c r="D9" s="1">
         <v>429.05200000000002</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>542.84299999999996</v>
       </c>
-      <c r="F9" s="4"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
@@ -600,10 +603,10 @@
       <c r="D10" s="1">
         <v>452.78899999999999</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>438.404</v>
       </c>
-      <c r="F10" s="4"/>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
@@ -618,10 +621,10 @@
       <c r="D11" s="1">
         <v>483.476</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="5">
         <v>383.30099999999999</v>
       </c>
-      <c r="F11" s="4"/>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
@@ -636,18 +639,18 @@
       <c r="D12" s="1">
         <v>518.16300000000001</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="5">
         <v>328.88</v>
       </c>
-      <c r="F12" s="4"/>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
+      <c r="A13" s="6"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Make hellwig great again
</commit_message>
<xml_diff>
--- a/dane.xlsx
+++ b/dane.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\Ekonometry\Ekonometry\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A40266D-2479-4EF8-8362-CB561DA7624B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E1081B0-3C32-473D-AC21-F7FB635A8DD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13740" yWindow="1950" windowWidth="13890" windowHeight="13650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="13890" windowHeight="13650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="date" sheetId="1" r:id="rId1"/>
@@ -113,7 +113,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -129,6 +129,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -418,28 +421,28 @@
   <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="4">

</xml_diff>